<commit_message>
Bug fixes and changes on convert_raw_stock_data method
</commit_message>
<xml_diff>
--- a/Data/stock_data.xlsx
+++ b/Data/stock_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\NTUT\Other\113IFM_camp\IFM_camp_bot\Bot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B434D555-BF21-4F0A-95E2-2C1D78A50AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327C8B7F-0A1B-46EF-A70E-24ABD9736169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F8FD49BE-BC86-4C92-8F4D-99B84D176403}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{F8FD49BE-BC86-4C92-8F4D-99B84D176403}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_data" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="42">
   <si>
     <t>base_period_eps</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -301,7 +301,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -341,6 +341,27 @@
     <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -359,44 +380,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -735,7 +720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A5B1930-18B5-46DE-91AC-AB66E4E6FDB4}">
   <dimension ref="A1:AI12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="G21" sqref="G21"/>
     </sheetView>
@@ -745,7 +730,7 @@
     <col min="1" max="1" width="12.125" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.75" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.625" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.625" style="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.75" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.625" style="1" bestFit="1" customWidth="1"/>
@@ -781,72 +766,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="16.5" customHeight="1">
-      <c r="A1" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="16" t="s">
+      <c r="A1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="14" t="s">
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="14" t="s">
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
-      <c r="AB1" s="15"/>
-      <c r="AC1" s="14" t="s">
+      <c r="W1" s="21"/>
+      <c r="X1" s="21"/>
+      <c r="Y1" s="21"/>
+      <c r="Z1" s="21"/>
+      <c r="AA1" s="21"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="AD1" s="14"/>
-      <c r="AE1" s="14"/>
-      <c r="AF1" s="14"/>
-      <c r="AG1" s="14"/>
-      <c r="AH1" s="14"/>
-      <c r="AI1" s="15"/>
+      <c r="AD1" s="21"/>
+      <c r="AE1" s="21"/>
+      <c r="AF1" s="21"/>
+      <c r="AG1" s="21"/>
+      <c r="AH1" s="21"/>
+      <c r="AI1" s="22"/>
     </row>
     <row r="2" spans="1:35" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="16"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="23"/>
       <c r="H2" s="8" t="s">
         <v>26</v>
       </c>
@@ -942,7 +927,7 @@
       <c r="C3" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="15">
         <v>1</v>
       </c>
       <c r="E3" s="6">
@@ -962,7 +947,7 @@
         <f>ROUND((H3-G3)/ABS(G3),4)</f>
         <v>0.125</v>
       </c>
-      <c r="J3" s="19">
+      <c r="J3" s="13">
         <v>1</v>
       </c>
       <c r="K3" s="12">
@@ -985,7 +970,7 @@
         <f>ROUND((O3-H3)/ABS(H3),4)</f>
         <v>0.16669999999999999</v>
       </c>
-      <c r="Q3" s="19">
+      <c r="Q3" s="13">
         <v>1</v>
       </c>
       <c r="R3" s="12">
@@ -1008,7 +993,7 @@
         <f>ROUND((V3-O3)/ABS(O3),4)</f>
         <v>-0.47620000000000001</v>
       </c>
-      <c r="X3" s="19">
+      <c r="X3" s="13">
         <v>1</v>
       </c>
       <c r="Y3" s="12">
@@ -1031,7 +1016,7 @@
         <f>ROUND((AC3-V3)/ABS(V3),4)</f>
         <v>1</v>
       </c>
-      <c r="AE3" s="19">
+      <c r="AE3" s="13">
         <v>1</v>
       </c>
       <c r="AF3" s="12">
@@ -1057,7 +1042,7 @@
       <c r="C4" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="15">
         <v>1</v>
       </c>
       <c r="E4" s="6">
@@ -1070,14 +1055,14 @@
         <v>7</v>
       </c>
       <c r="H4" s="9">
-        <f t="shared" ref="H4:H12" si="0">N4/$F4</f>
+        <f t="shared" ref="H4:H11" si="0">N4/$F4</f>
         <v>7.5</v>
       </c>
       <c r="I4" s="11">
         <f t="shared" ref="I4:I12" si="1">ROUND((H4-G4)/ABS(G4),4)</f>
         <v>7.1400000000000005E-2</v>
       </c>
-      <c r="J4" s="19">
+      <c r="J4" s="13">
         <v>1</v>
       </c>
       <c r="K4" s="12">
@@ -1100,7 +1085,7 @@
         <f t="shared" ref="P4:P12" si="3">ROUND((O4-H4)/ABS(H4),4)</f>
         <v>0.2</v>
       </c>
-      <c r="Q4" s="19">
+      <c r="Q4" s="13">
         <v>1</v>
       </c>
       <c r="R4" s="12">
@@ -1123,7 +1108,7 @@
         <f t="shared" ref="W4:W12" si="5">ROUND((V4-O4)/ABS(O4),4)</f>
         <v>-8.3299999999999999E-2</v>
       </c>
-      <c r="X4" s="19">
+      <c r="X4" s="13">
         <v>1</v>
       </c>
       <c r="Y4" s="12">
@@ -1146,7 +1131,7 @@
         <f t="shared" ref="AD4:AD12" si="7">ROUND((AC4-V4)/ABS(V4),4)</f>
         <v>0.39389999999999997</v>
       </c>
-      <c r="AE4" s="19">
+      <c r="AE4" s="13">
         <v>1</v>
       </c>
       <c r="AF4" s="12">
@@ -1172,7 +1157,7 @@
       <c r="C5" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="15">
         <v>1</v>
       </c>
       <c r="E5" s="6">
@@ -1192,7 +1177,7 @@
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="J5" s="19">
+      <c r="J5" s="13">
         <v>1</v>
       </c>
       <c r="K5" s="12">
@@ -1215,7 +1200,7 @@
         <f t="shared" si="3"/>
         <v>-1.0909</v>
       </c>
-      <c r="Q5" s="19">
+      <c r="Q5" s="13">
         <v>1</v>
       </c>
       <c r="R5" s="12">
@@ -1238,7 +1223,7 @@
         <f t="shared" si="5"/>
         <v>-3</v>
       </c>
-      <c r="X5" s="19">
+      <c r="X5" s="13">
         <v>1</v>
       </c>
       <c r="Y5" s="12">
@@ -1261,7 +1246,7 @@
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
-      <c r="AE5" s="19">
+      <c r="AE5" s="13">
         <v>1</v>
       </c>
       <c r="AF5" s="12">
@@ -1287,7 +1272,7 @@
       <c r="C6" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="15">
         <v>1</v>
       </c>
       <c r="E6" s="6">
@@ -1307,7 +1292,7 @@
         <f t="shared" si="1"/>
         <v>7.1400000000000005E-2</v>
       </c>
-      <c r="J6" s="19">
+      <c r="J6" s="13">
         <v>1</v>
       </c>
       <c r="K6" s="12">
@@ -1330,7 +1315,7 @@
         <f t="shared" si="3"/>
         <v>0.31669999999999998</v>
       </c>
-      <c r="Q6" s="19">
+      <c r="Q6" s="13">
         <v>1</v>
       </c>
       <c r="R6" s="12">
@@ -1353,7 +1338,7 @@
         <f t="shared" si="5"/>
         <v>-0.50629999999999997</v>
       </c>
-      <c r="X6" s="19">
+      <c r="X6" s="13">
         <v>1</v>
       </c>
       <c r="Y6" s="12">
@@ -1376,7 +1361,7 @@
         <f t="shared" si="7"/>
         <v>1.1026</v>
       </c>
-      <c r="AE6" s="19">
+      <c r="AE6" s="13">
         <v>1</v>
       </c>
       <c r="AF6" s="12">
@@ -1402,7 +1387,7 @@
       <c r="C7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="15">
         <v>1</v>
       </c>
       <c r="E7" s="6">
@@ -1422,7 +1407,7 @@
         <f t="shared" si="1"/>
         <v>-0.1211</v>
       </c>
-      <c r="J7" s="19">
+      <c r="J7" s="13">
         <v>1</v>
       </c>
       <c r="K7" s="12">
@@ -1445,7 +1430,7 @@
         <f t="shared" si="3"/>
         <v>-9.0300000000000005E-2</v>
       </c>
-      <c r="Q7" s="19">
+      <c r="Q7" s="13">
         <v>1</v>
       </c>
       <c r="R7" s="12">
@@ -1468,7 +1453,7 @@
         <f t="shared" si="5"/>
         <v>-1.7899999999999999E-2</v>
       </c>
-      <c r="X7" s="19">
+      <c r="X7" s="13">
         <v>1</v>
       </c>
       <c r="Y7" s="12">
@@ -1491,7 +1476,7 @@
         <f t="shared" si="7"/>
         <v>9.0899999999999995E-2</v>
       </c>
-      <c r="AE7" s="19">
+      <c r="AE7" s="13">
         <v>1</v>
       </c>
       <c r="AF7" s="12">
@@ -1517,7 +1502,7 @@
       <c r="C8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D8" s="15">
         <v>1</v>
       </c>
       <c r="E8" s="6">
@@ -1537,7 +1522,7 @@
         <f t="shared" si="1"/>
         <v>5.8799999999999998E-2</v>
       </c>
-      <c r="J8" s="19">
+      <c r="J8" s="13">
         <v>1</v>
       </c>
       <c r="K8" s="12">
@@ -1560,7 +1545,7 @@
         <f t="shared" si="3"/>
         <v>0.77410000000000001</v>
       </c>
-      <c r="Q8" s="19">
+      <c r="Q8" s="13">
         <v>1</v>
       </c>
       <c r="R8" s="12">
@@ -1583,7 +1568,7 @@
         <f t="shared" si="5"/>
         <v>-0.16489999999999999</v>
       </c>
-      <c r="X8" s="19">
+      <c r="X8" s="13">
         <v>1</v>
       </c>
       <c r="Y8" s="12">
@@ -1606,7 +1591,7 @@
         <f t="shared" si="7"/>
         <v>-1.2500000000000001E-2</v>
       </c>
-      <c r="AE8" s="19">
+      <c r="AE8" s="13">
         <v>1</v>
       </c>
       <c r="AF8" s="12">
@@ -1632,7 +1617,7 @@
       <c r="C9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="15">
         <v>1</v>
       </c>
       <c r="E9" s="6">
@@ -1652,7 +1637,7 @@
         <f t="shared" si="1"/>
         <v>-0.1237</v>
       </c>
-      <c r="J9" s="19">
+      <c r="J9" s="13">
         <v>1</v>
       </c>
       <c r="K9" s="12">
@@ -1675,7 +1660,7 @@
         <f t="shared" si="3"/>
         <v>0.45590000000000003</v>
       </c>
-      <c r="Q9" s="19">
+      <c r="Q9" s="13">
         <v>1</v>
       </c>
       <c r="R9" s="12">
@@ -1698,7 +1683,7 @@
         <f t="shared" si="5"/>
         <v>0.1414</v>
       </c>
-      <c r="X9" s="19">
+      <c r="X9" s="13">
         <v>1</v>
       </c>
       <c r="Y9" s="12">
@@ -1721,7 +1706,7 @@
         <f t="shared" si="7"/>
         <v>0.1381</v>
       </c>
-      <c r="AE9" s="19">
+      <c r="AE9" s="13">
         <v>1</v>
       </c>
       <c r="AF9" s="12">
@@ -1747,7 +1732,7 @@
       <c r="C10" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D10" s="15">
         <v>1</v>
       </c>
       <c r="E10" s="6">
@@ -1767,7 +1752,7 @@
         <f t="shared" si="1"/>
         <v>3.4500000000000003E-2</v>
       </c>
-      <c r="J10" s="19">
+      <c r="J10" s="13">
         <v>1</v>
       </c>
       <c r="K10" s="12">
@@ -1790,7 +1775,7 @@
         <f t="shared" si="3"/>
         <v>-1.0432999999999999</v>
       </c>
-      <c r="Q10" s="19">
+      <c r="Q10" s="13">
         <v>1</v>
       </c>
       <c r="R10" s="12">
@@ -1813,7 +1798,7 @@
         <f t="shared" si="5"/>
         <v>12.538500000000001</v>
       </c>
-      <c r="X10" s="19">
+      <c r="X10" s="13">
         <v>1</v>
       </c>
       <c r="Y10" s="12">
@@ -1836,7 +1821,7 @@
         <f t="shared" si="7"/>
         <v>1.52</v>
       </c>
-      <c r="AE10" s="19">
+      <c r="AE10" s="13">
         <v>1</v>
       </c>
       <c r="AF10" s="12">
@@ -1862,7 +1847,7 @@
       <c r="C11" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="15">
         <v>1</v>
       </c>
       <c r="E11" s="6">
@@ -1882,7 +1867,7 @@
         <f t="shared" si="1"/>
         <v>2.5600000000000001E-2</v>
       </c>
-      <c r="J11" s="19">
+      <c r="J11" s="13">
         <v>1</v>
       </c>
       <c r="K11" s="12">
@@ -1905,7 +1890,7 @@
         <f t="shared" si="3"/>
         <v>3.3300000000000003E-2</v>
       </c>
-      <c r="Q11" s="19">
+      <c r="Q11" s="13">
         <v>1</v>
       </c>
       <c r="R11" s="12">
@@ -1928,7 +1913,7 @@
         <f t="shared" si="5"/>
         <v>-8.0999999999999996E-3</v>
       </c>
-      <c r="X11" s="19">
+      <c r="X11" s="13">
         <v>1</v>
       </c>
       <c r="Y11" s="12">
@@ -1951,7 +1936,7 @@
         <f t="shared" si="7"/>
         <v>5.6899999999999999E-2</v>
       </c>
-      <c r="AE11" s="19">
+      <c r="AE11" s="13">
         <v>1</v>
       </c>
       <c r="AF11" s="12">
@@ -1977,7 +1962,7 @@
       <c r="C12" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="15">
         <v>1</v>
       </c>
       <c r="E12" s="6">
@@ -1997,7 +1982,7 @@
         <f t="shared" si="1"/>
         <v>5.67E-2</v>
       </c>
-      <c r="J12" s="19">
+      <c r="J12" s="13">
         <v>1</v>
       </c>
       <c r="K12" s="12">
@@ -2020,7 +2005,7 @@
         <f t="shared" si="3"/>
         <v>3.3099999999999997E-2</v>
       </c>
-      <c r="Q12" s="19">
+      <c r="Q12" s="13">
         <v>1</v>
       </c>
       <c r="R12" s="12">
@@ -2043,7 +2028,7 @@
         <f t="shared" si="5"/>
         <v>3.5099999999999999E-2</v>
       </c>
-      <c r="X12" s="19">
+      <c r="X12" s="13">
         <v>1</v>
       </c>
       <c r="Y12" s="12">
@@ -2066,7 +2051,7 @@
         <f t="shared" si="7"/>
         <v>1.77E-2</v>
       </c>
-      <c r="AE12" s="19">
+      <c r="AE12" s="13">
         <v>1</v>
       </c>
       <c r="AF12" s="12">
@@ -2106,7 +2091,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D11"/>
+      <selection activeCell="B2" sqref="B2:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2141,7 +2126,7 @@
       <c r="C2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="2">
         <f>raw_data!E3</f>
         <v>30</v>
       </c>
@@ -2156,7 +2141,7 @@
       <c r="C3" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="2">
         <f>raw_data!E4</f>
         <v>15</v>
       </c>
@@ -2171,7 +2156,7 @@
       <c r="C4" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="2">
         <f>raw_data!E5</f>
         <v>10</v>
       </c>
@@ -2186,7 +2171,7 @@
       <c r="C5" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="2">
         <f>raw_data!E6</f>
         <v>25</v>
       </c>
@@ -2201,7 +2186,7 @@
       <c r="C6" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="2">
         <f>raw_data!E7</f>
         <v>7</v>
       </c>
@@ -2216,7 +2201,7 @@
       <c r="C7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="2">
         <f>raw_data!E8</f>
         <v>5</v>
       </c>
@@ -2231,7 +2216,7 @@
       <c r="C8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="2">
         <f>raw_data!E9</f>
         <v>8</v>
       </c>
@@ -2246,7 +2231,7 @@
       <c r="C9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="2">
         <f>raw_data!E10</f>
         <v>6</v>
       </c>
@@ -2261,7 +2246,7 @@
       <c r="C10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="2">
         <f>raw_data!E11</f>
         <v>9</v>
       </c>
@@ -2276,7 +2261,7 @@
       <c r="C11" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="2">
         <f>raw_data!E12</f>
         <v>10</v>
       </c>
@@ -2289,392 +2274,425 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90C12C4C-BD75-4062-B27A-BB09B9B8FD6C}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="C1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="E1" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="30">
+    <row r="2" spans="1:9">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="15">
         <f>raw_data!D3</f>
         <v>1</v>
       </c>
-      <c r="B2" s="28">
+      <c r="C2" s="2">
         <f>raw_data!H3</f>
         <v>18</v>
       </c>
-      <c r="C2" s="20">
+      <c r="D2" s="14">
         <f>raw_data!I3</f>
         <v>0.125</v>
       </c>
-      <c r="D2" s="20">
+      <c r="E2" s="14">
         <f>raw_data!J3</f>
         <v>1</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <f>raw_data!K3</f>
         <v>9000000</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <f>raw_data!L3</f>
         <v>5000000</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <f>raw_data!M3</f>
         <v>4100000</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I2" s="2">
         <f>raw_data!N3</f>
         <v>3600000</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="30">
+    <row r="3" spans="1:9">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="15">
         <f>raw_data!D4</f>
         <v>1</v>
       </c>
-      <c r="B3" s="28">
+      <c r="C3" s="2">
         <f>raw_data!H4</f>
         <v>7.5</v>
       </c>
-      <c r="C3" s="20">
+      <c r="D3" s="14">
         <f>raw_data!I4</f>
         <v>7.1400000000000005E-2</v>
       </c>
-      <c r="D3" s="20">
+      <c r="E3" s="14">
         <f>raw_data!J4</f>
         <v>1</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <f>raw_data!K4</f>
         <v>4000000</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <f>raw_data!L4</f>
         <v>2500000</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <f>raw_data!M4</f>
         <v>2000000</v>
       </c>
-      <c r="H3" s="2">
+      <c r="I3" s="2">
         <f>raw_data!N4</f>
         <v>1500000</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="30">
+    <row r="4" spans="1:9">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="15">
         <f>raw_data!D5</f>
         <v>1</v>
       </c>
-      <c r="B4" s="28">
+      <c r="C4" s="2">
         <f>raw_data!H5</f>
         <v>5.5</v>
       </c>
-      <c r="C4" s="20">
+      <c r="D4" s="14">
         <f>raw_data!I5</f>
         <v>0.1</v>
       </c>
-      <c r="D4" s="20">
+      <c r="E4" s="14">
         <f>raw_data!J5</f>
         <v>1</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <f>raw_data!K5</f>
         <v>4500000</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <f>raw_data!L5</f>
         <v>2400000</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <f>raw_data!M5</f>
         <v>1900000</v>
       </c>
-      <c r="H4" s="2">
+      <c r="I4" s="2">
         <f>raw_data!N5</f>
         <v>1100000</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="30">
+    <row r="5" spans="1:9">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="15">
         <f>raw_data!D6</f>
         <v>1</v>
       </c>
-      <c r="B5" s="28">
+      <c r="C5" s="2">
         <f>raw_data!H6</f>
         <v>15</v>
       </c>
-      <c r="C5" s="20">
+      <c r="D5" s="14">
         <f>raw_data!I6</f>
         <v>7.1400000000000005E-2</v>
       </c>
-      <c r="D5" s="20">
+      <c r="E5" s="14">
         <f>raw_data!J6</f>
         <v>1</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <f>raw_data!K6</f>
         <v>8200000</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <f>raw_data!L6</f>
         <v>6200000</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <f>raw_data!M6</f>
         <v>4000000</v>
       </c>
-      <c r="H5" s="2">
+      <c r="I5" s="2">
         <f>raw_data!N6</f>
         <v>3000000</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="30">
+    <row r="6" spans="1:9">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="15">
         <f>raw_data!D7</f>
         <v>1</v>
       </c>
-      <c r="B6" s="28">
+      <c r="C6" s="2">
         <f>raw_data!H7</f>
         <v>1.5389999999999999</v>
       </c>
-      <c r="C6" s="20">
+      <c r="D6" s="14">
         <f>raw_data!I7</f>
         <v>-0.1211</v>
       </c>
-      <c r="D6" s="20">
+      <c r="E6" s="14">
         <f>raw_data!J7</f>
         <v>1</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <f>raw_data!K7</f>
         <v>600000</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <f>raw_data!L7</f>
         <v>440000</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <f>raw_data!M7</f>
         <v>390000</v>
       </c>
-      <c r="H6" s="2">
+      <c r="I6" s="2">
         <f>raw_data!N7</f>
         <v>307800</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="30">
+    <row r="7" spans="1:9">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="15">
         <f>raw_data!D8</f>
         <v>1</v>
       </c>
-      <c r="B7" s="28">
+      <c r="C7" s="2">
         <f>raw_data!H8</f>
         <v>1.35</v>
       </c>
-      <c r="C7" s="20">
+      <c r="D7" s="14">
         <f>raw_data!I8</f>
         <v>5.8799999999999998E-2</v>
       </c>
-      <c r="D7" s="20">
+      <c r="E7" s="14">
         <f>raw_data!J8</f>
         <v>1</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <f>raw_data!K8</f>
         <v>500000</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7" s="2">
         <f>raw_data!L8</f>
         <v>380000</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="2">
         <f>raw_data!M8</f>
         <v>320000</v>
       </c>
-      <c r="H7" s="2">
+      <c r="I7" s="2">
         <f>raw_data!N8</f>
         <v>270000</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="30">
+    <row r="8" spans="1:9">
+      <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="15">
         <f>raw_data!D9</f>
         <v>1</v>
       </c>
-      <c r="B8" s="28">
+      <c r="C8" s="2">
         <f>raw_data!H9</f>
         <v>1.7</v>
       </c>
-      <c r="C8" s="20">
+      <c r="D8" s="14">
         <f>raw_data!I9</f>
         <v>-0.1237</v>
       </c>
-      <c r="D8" s="20">
+      <c r="E8" s="14">
         <f>raw_data!J9</f>
         <v>1</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <f>raw_data!K9</f>
         <v>700000</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <f>raw_data!L9</f>
         <v>500000</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <f>raw_data!M9</f>
         <v>400000</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I8" s="2">
         <f>raw_data!N9</f>
         <v>340000</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="30">
+    <row r="9" spans="1:9">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="15">
         <f>raw_data!D10</f>
         <v>1</v>
       </c>
-      <c r="B9" s="28">
+      <c r="C9" s="2">
         <f>raw_data!H10</f>
         <v>1.5</v>
       </c>
-      <c r="C9" s="20">
+      <c r="D9" s="14">
         <f>raw_data!I10</f>
         <v>3.4500000000000003E-2</v>
       </c>
-      <c r="D9" s="20">
+      <c r="E9" s="14">
         <f>raw_data!J10</f>
         <v>1</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <f>raw_data!K10</f>
         <v>640000</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G9" s="2">
         <f>raw_data!L10</f>
         <v>550000</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H9" s="2">
         <f>raw_data!M10</f>
         <v>470000</v>
       </c>
-      <c r="H9" s="2">
+      <c r="I9" s="2">
         <f>raw_data!N10</f>
         <v>300000</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="30">
+    <row r="10" spans="1:9">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="15">
         <f>raw_data!D11</f>
         <v>1</v>
       </c>
-      <c r="B10" s="28">
+      <c r="C10" s="2">
         <f>raw_data!H11</f>
         <v>0.6</v>
       </c>
-      <c r="C10" s="20">
+      <c r="D10" s="14">
         <f>raw_data!I11</f>
         <v>2.5600000000000001E-2</v>
       </c>
-      <c r="D10" s="20">
+      <c r="E10" s="14">
         <f>raw_data!J11</f>
         <v>1</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F10" s="2">
         <f>raw_data!K11</f>
         <v>800000</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G10" s="2">
         <f>raw_data!L11</f>
         <v>750000</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" s="2">
         <f>raw_data!M11</f>
         <v>650000</v>
       </c>
-      <c r="H10" s="2">
+      <c r="I10" s="2">
         <f>raw_data!N11</f>
         <v>600000</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="30">
+    <row r="11" spans="1:9">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="15">
         <f>raw_data!D12</f>
         <v>1</v>
       </c>
-      <c r="B11" s="28">
+      <c r="C11" s="2">
         <f>raw_data!H12</f>
         <v>0.63400000000000001</v>
       </c>
-      <c r="C11" s="20">
+      <c r="D11" s="14">
         <f>raw_data!I12</f>
         <v>5.67E-2</v>
       </c>
-      <c r="D11" s="20">
+      <c r="E11" s="14">
         <f>raw_data!J12</f>
         <v>1</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F11" s="2">
         <f>raw_data!K12</f>
         <v>815000</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G11" s="2">
         <f>raw_data!L12</f>
         <v>770000</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H11" s="2">
         <f>raw_data!M12</f>
         <v>685000</v>
       </c>
-      <c r="H11" s="2">
+      <c r="I11" s="2">
         <f>raw_data!N12</f>
         <v>634000</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="24"/>
+    <row r="12" spans="1:9">
+      <c r="B12" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2684,384 +2702,420 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E2A3E3-92D7-4292-A795-B0C68BB6C50D}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="C1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="E1" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="30">
+    <row r="2" spans="1:9">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="15">
         <f>raw_data!D3</f>
         <v>1</v>
       </c>
-      <c r="B2" s="28">
+      <c r="C2" s="2">
         <f>raw_data!O3</f>
         <v>21</v>
       </c>
-      <c r="C2" s="28">
+      <c r="D2" s="2">
         <f>raw_data!P3</f>
         <v>0.16669999999999999</v>
       </c>
-      <c r="D2" s="31">
+      <c r="E2" s="14">
         <f>raw_data!Q3</f>
         <v>1</v>
       </c>
-      <c r="E2" s="28">
+      <c r="F2" s="2">
         <f>raw_data!R3</f>
         <v>10000000</v>
       </c>
-      <c r="F2" s="28">
+      <c r="G2" s="2">
         <f>raw_data!S3</f>
         <v>6500000</v>
       </c>
-      <c r="G2" s="28">
+      <c r="H2" s="2">
         <f>raw_data!T3</f>
         <v>5000000</v>
       </c>
-      <c r="H2" s="28">
+      <c r="I2" s="2">
         <f>raw_data!U3</f>
         <v>4200000</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="30">
+    <row r="3" spans="1:9">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="15">
         <f>raw_data!D4</f>
         <v>1</v>
       </c>
-      <c r="B3" s="28">
+      <c r="C3" s="2">
         <f>raw_data!O4</f>
         <v>9</v>
       </c>
-      <c r="C3" s="28">
+      <c r="D3" s="2">
         <f>raw_data!P4</f>
         <v>0.2</v>
       </c>
-      <c r="D3" s="31">
+      <c r="E3" s="14">
         <f>raw_data!Q4</f>
         <v>1</v>
       </c>
-      <c r="E3" s="28">
+      <c r="F3" s="2">
         <f>raw_data!R4</f>
         <v>4500000</v>
       </c>
-      <c r="F3" s="28">
+      <c r="G3" s="2">
         <f>raw_data!S4</f>
         <v>3000000</v>
       </c>
-      <c r="G3" s="28">
+      <c r="H3" s="2">
         <f>raw_data!T4</f>
         <v>2000000</v>
       </c>
-      <c r="H3" s="28">
+      <c r="I3" s="2">
         <f>raw_data!U4</f>
         <v>1800000</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="30">
+    <row r="4" spans="1:9">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="15">
         <f>raw_data!D5</f>
         <v>1</v>
       </c>
-      <c r="B4" s="28">
+      <c r="C4" s="2">
         <f>raw_data!O5</f>
         <v>-0.5</v>
       </c>
-      <c r="C4" s="28">
+      <c r="D4" s="2">
         <f>raw_data!P5</f>
         <v>-1.0909</v>
       </c>
-      <c r="D4" s="31">
+      <c r="E4" s="14">
         <f>raw_data!Q5</f>
         <v>1</v>
       </c>
-      <c r="E4" s="28">
+      <c r="F4" s="2">
         <f>raw_data!R5</f>
         <v>2500000</v>
       </c>
-      <c r="F4" s="28">
+      <c r="G4" s="2">
         <f>raw_data!S5</f>
         <v>1000000</v>
       </c>
-      <c r="G4" s="28">
+      <c r="H4" s="2">
         <f>raw_data!T5</f>
         <v>200000</v>
       </c>
-      <c r="H4" s="28">
+      <c r="I4" s="2">
         <f>raw_data!U5</f>
         <v>-100000</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="30">
+    <row r="5" spans="1:9">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="15">
         <f>raw_data!D6</f>
         <v>1</v>
       </c>
-      <c r="B5" s="28">
+      <c r="C5" s="2">
         <f>raw_data!O6</f>
         <v>19.75</v>
       </c>
-      <c r="C5" s="28">
+      <c r="D5" s="2">
         <f>raw_data!P6</f>
         <v>0.31669999999999998</v>
       </c>
-      <c r="D5" s="31">
+      <c r="E5" s="14">
         <f>raw_data!Q6</f>
         <v>1</v>
       </c>
-      <c r="E5" s="28">
+      <c r="F5" s="2">
         <f>raw_data!R6</f>
         <v>9500000</v>
       </c>
-      <c r="F5" s="28">
+      <c r="G5" s="2">
         <f>raw_data!S6</f>
         <v>7800000</v>
       </c>
-      <c r="G5" s="28">
+      <c r="H5" s="2">
         <f>raw_data!T6</f>
         <v>6350000</v>
       </c>
-      <c r="H5" s="28">
+      <c r="I5" s="2">
         <f>raw_data!U6</f>
         <v>3950000</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="30">
+    <row r="6" spans="1:9">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="15">
         <f>raw_data!D7</f>
         <v>1</v>
       </c>
-      <c r="B6" s="28">
+      <c r="C6" s="2">
         <f>raw_data!O7</f>
         <v>1.4</v>
       </c>
-      <c r="C6" s="28">
+      <c r="D6" s="2">
         <f>raw_data!P7</f>
         <v>-9.0300000000000005E-2</v>
       </c>
-      <c r="D6" s="31">
+      <c r="E6" s="14">
         <f>raw_data!Q7</f>
         <v>1</v>
       </c>
-      <c r="E6" s="28">
+      <c r="F6" s="2">
         <f>raw_data!R7</f>
         <v>450000</v>
       </c>
-      <c r="F6" s="28">
+      <c r="G6" s="2">
         <f>raw_data!S7</f>
         <v>390000</v>
       </c>
-      <c r="G6" s="28">
+      <c r="H6" s="2">
         <f>raw_data!T7</f>
         <v>320000</v>
       </c>
-      <c r="H6" s="28">
+      <c r="I6" s="2">
         <f>raw_data!U7</f>
         <v>280000</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="30">
+    <row r="7" spans="1:9">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="15">
         <f>raw_data!D8</f>
         <v>1</v>
       </c>
-      <c r="B7" s="28">
+      <c r="C7" s="2">
         <f>raw_data!O8</f>
         <v>2.395</v>
       </c>
-      <c r="C7" s="28">
+      <c r="D7" s="2">
         <f>raw_data!P8</f>
         <v>0.77410000000000001</v>
       </c>
-      <c r="D7" s="31">
+      <c r="E7" s="14">
         <f>raw_data!Q8</f>
         <v>1</v>
       </c>
-      <c r="E7" s="28">
+      <c r="F7" s="2">
         <f>raw_data!R8</f>
         <v>650000</v>
       </c>
-      <c r="F7" s="28">
+      <c r="G7" s="2">
         <f>raw_data!S8</f>
         <v>570000</v>
       </c>
-      <c r="G7" s="28">
+      <c r="H7" s="2">
         <f>raw_data!T8</f>
         <v>500000</v>
       </c>
-      <c r="H7" s="28">
+      <c r="I7" s="2">
         <f>raw_data!U8</f>
         <v>479000</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="30">
+    <row r="8" spans="1:9">
+      <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="15">
         <f>raw_data!D9</f>
         <v>1</v>
       </c>
-      <c r="B8" s="28">
+      <c r="C8" s="2">
         <f>raw_data!O9</f>
         <v>2.4750000000000001</v>
       </c>
-      <c r="C8" s="28">
+      <c r="D8" s="2">
         <f>raw_data!P9</f>
         <v>0.45590000000000003</v>
       </c>
-      <c r="D8" s="31">
+      <c r="E8" s="14">
         <f>raw_data!Q9</f>
         <v>1</v>
       </c>
-      <c r="E8" s="28">
+      <c r="F8" s="2">
         <f>raw_data!R9</f>
         <v>1100000</v>
       </c>
-      <c r="F8" s="28">
+      <c r="G8" s="2">
         <f>raw_data!S9</f>
         <v>750000</v>
       </c>
-      <c r="G8" s="28">
+      <c r="H8" s="2">
         <f>raw_data!T9</f>
         <v>558000</v>
       </c>
-      <c r="H8" s="28">
+      <c r="I8" s="2">
         <f>raw_data!U9</f>
         <v>495000</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="30">
+    <row r="9" spans="1:9">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="15">
         <f>raw_data!D10</f>
         <v>1</v>
       </c>
-      <c r="B9" s="28">
+      <c r="C9" s="2">
         <f>raw_data!O10</f>
         <v>-6.5000000000000002E-2</v>
       </c>
-      <c r="C9" s="28">
+      <c r="D9" s="2">
         <f>raw_data!P10</f>
         <v>-1.0432999999999999</v>
       </c>
-      <c r="D9" s="31">
+      <c r="E9" s="14">
         <f>raw_data!Q10</f>
         <v>1</v>
       </c>
-      <c r="E9" s="28">
+      <c r="F9" s="2">
         <f>raw_data!R10</f>
         <v>470610</v>
       </c>
-      <c r="F9" s="28">
+      <c r="G9" s="2">
         <f>raw_data!S10</f>
         <v>250000</v>
       </c>
-      <c r="G9" s="28">
+      <c r="H9" s="2">
         <f>raw_data!T10</f>
         <v>110000</v>
       </c>
-      <c r="H9" s="28">
+      <c r="I9" s="2">
         <f>raw_data!U10</f>
         <v>-13000</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="30">
+    <row r="10" spans="1:9">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="15">
         <f>raw_data!D11</f>
         <v>1</v>
       </c>
-      <c r="B10" s="28">
+      <c r="C10" s="2">
         <f>raw_data!O11</f>
         <v>0.62</v>
       </c>
-      <c r="C10" s="28">
+      <c r="D10" s="2">
         <f>raw_data!P11</f>
         <v>3.3300000000000003E-2</v>
       </c>
-      <c r="D10" s="31">
+      <c r="E10" s="14">
         <f>raw_data!Q11</f>
         <v>1</v>
       </c>
-      <c r="E10" s="28">
+      <c r="F10" s="2">
         <f>raw_data!R11</f>
         <v>810000</v>
       </c>
-      <c r="F10" s="28">
+      <c r="G10" s="2">
         <f>raw_data!S11</f>
         <v>740000</v>
       </c>
-      <c r="G10" s="28">
+      <c r="H10" s="2">
         <f>raw_data!T11</f>
         <v>660000</v>
       </c>
-      <c r="H10" s="28">
+      <c r="I10" s="2">
         <f>raw_data!U11</f>
         <v>620000</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="30">
+    <row r="11" spans="1:9">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="15">
         <f>raw_data!D12</f>
         <v>1</v>
       </c>
-      <c r="B11" s="28">
+      <c r="C11" s="2">
         <f>raw_data!O12</f>
         <v>0.65500000000000003</v>
       </c>
-      <c r="C11" s="28">
+      <c r="D11" s="2">
         <f>raw_data!P12</f>
         <v>3.3099999999999997E-2</v>
       </c>
-      <c r="D11" s="31">
+      <c r="E11" s="14">
         <f>raw_data!Q12</f>
         <v>1</v>
       </c>
-      <c r="E11" s="28">
+      <c r="F11" s="2">
         <f>raw_data!R12</f>
         <v>820000</v>
       </c>
-      <c r="F11" s="28">
+      <c r="G11" s="2">
         <f>raw_data!S12</f>
         <v>778000</v>
       </c>
-      <c r="G11" s="28">
+      <c r="H11" s="2">
         <f>raw_data!T12</f>
         <v>700000</v>
       </c>
-      <c r="H11" s="28">
+      <c r="I11" s="2">
         <f>raw_data!U12</f>
         <v>655000</v>
       </c>
@@ -3074,384 +3128,420 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5A42A6B-97CE-4851-AF52-314A8693FFD1}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="C1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="E1" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="30">
+    <row r="2" spans="1:9">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="15">
         <f>raw_data!D3</f>
         <v>1</v>
       </c>
-      <c r="B2" s="28">
+      <c r="C2" s="2">
         <f>raw_data!V3</f>
         <v>11</v>
       </c>
-      <c r="C2" s="28">
+      <c r="D2" s="2">
         <f>raw_data!W3</f>
         <v>-0.47620000000000001</v>
       </c>
-      <c r="D2" s="31">
+      <c r="E2" s="14">
         <f>raw_data!X3</f>
         <v>1</v>
       </c>
-      <c r="E2" s="28">
+      <c r="F2" s="2">
         <f>raw_data!Y3</f>
         <v>8000000</v>
       </c>
-      <c r="F2" s="28">
+      <c r="G2" s="2">
         <f>raw_data!Z3</f>
         <v>4500000</v>
       </c>
-      <c r="G2" s="28">
+      <c r="H2" s="2">
         <f>raw_data!AA3</f>
         <v>2800000</v>
       </c>
-      <c r="H2" s="28">
+      <c r="I2" s="2">
         <f>raw_data!AB3</f>
         <v>2200000</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="30">
+    <row r="3" spans="1:9">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="15">
         <f>raw_data!D4</f>
         <v>1</v>
       </c>
-      <c r="B3" s="28">
+      <c r="C3" s="2">
         <f>raw_data!V4</f>
         <v>8.25</v>
       </c>
-      <c r="C3" s="28">
+      <c r="D3" s="2">
         <f>raw_data!W4</f>
         <v>-8.3299999999999999E-2</v>
       </c>
-      <c r="D3" s="31">
+      <c r="E3" s="14">
         <f>raw_data!X4</f>
         <v>1</v>
       </c>
-      <c r="E3" s="28">
+      <c r="F3" s="2">
         <f>raw_data!Y4</f>
         <v>3800000</v>
       </c>
-      <c r="F3" s="28">
+      <c r="G3" s="2">
         <f>raw_data!Z4</f>
         <v>2500000</v>
       </c>
-      <c r="G3" s="28">
+      <c r="H3" s="2">
         <f>raw_data!AA4</f>
         <v>1900000</v>
       </c>
-      <c r="H3" s="28">
+      <c r="I3" s="2">
         <f>raw_data!AB4</f>
         <v>1650000</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="30">
+    <row r="4" spans="1:9">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="15">
         <f>raw_data!D5</f>
         <v>1</v>
       </c>
-      <c r="B4" s="28">
+      <c r="C4" s="2">
         <f>raw_data!V5</f>
         <v>-2</v>
       </c>
-      <c r="C4" s="28">
+      <c r="D4" s="2">
         <f>raw_data!W5</f>
         <v>-3</v>
       </c>
-      <c r="D4" s="31">
+      <c r="E4" s="14">
         <f>raw_data!X5</f>
         <v>1</v>
       </c>
-      <c r="E4" s="28">
+      <c r="F4" s="2">
         <f>raw_data!Y5</f>
         <v>2000000</v>
       </c>
-      <c r="F4" s="28">
+      <c r="G4" s="2">
         <f>raw_data!Z5</f>
         <v>1250000</v>
       </c>
-      <c r="G4" s="28">
+      <c r="H4" s="2">
         <f>raw_data!AA5</f>
         <v>150000</v>
       </c>
-      <c r="H4" s="28">
+      <c r="I4" s="2">
         <f>raw_data!AB5</f>
         <v>-400000</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="30">
+    <row r="5" spans="1:9">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="15">
         <f>raw_data!D6</f>
         <v>1</v>
       </c>
-      <c r="B5" s="28">
+      <c r="C5" s="2">
         <f>raw_data!V6</f>
         <v>9.75</v>
       </c>
-      <c r="C5" s="28">
+      <c r="D5" s="2">
         <f>raw_data!W6</f>
         <v>-0.50629999999999997</v>
       </c>
-      <c r="D5" s="31">
+      <c r="E5" s="14">
         <f>raw_data!X6</f>
         <v>1</v>
       </c>
-      <c r="E5" s="28">
+      <c r="F5" s="2">
         <f>raw_data!Y6</f>
         <v>7900000</v>
       </c>
-      <c r="F5" s="28">
+      <c r="G5" s="2">
         <f>raw_data!Z6</f>
         <v>4000000</v>
       </c>
-      <c r="G5" s="28">
+      <c r="H5" s="2">
         <f>raw_data!AA6</f>
         <v>2600000</v>
       </c>
-      <c r="H5" s="28">
+      <c r="I5" s="2">
         <f>raw_data!AB6</f>
         <v>1950000</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="30">
+    <row r="6" spans="1:9">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="15">
         <f>raw_data!D7</f>
         <v>1</v>
       </c>
-      <c r="B6" s="28">
+      <c r="C6" s="2">
         <f>raw_data!V7</f>
         <v>1.375</v>
       </c>
-      <c r="C6" s="28">
+      <c r="D6" s="2">
         <f>raw_data!W7</f>
         <v>-1.7899999999999999E-2</v>
       </c>
-      <c r="D6" s="31">
+      <c r="E6" s="14">
         <f>raw_data!X7</f>
         <v>1</v>
       </c>
-      <c r="E6" s="28">
+      <c r="F6" s="2">
         <f>raw_data!Y7</f>
         <v>446000</v>
       </c>
-      <c r="F6" s="28">
+      <c r="G6" s="2">
         <f>raw_data!Z7</f>
         <v>360000</v>
       </c>
-      <c r="G6" s="28">
+      <c r="H6" s="2">
         <f>raw_data!AA7</f>
         <v>300000</v>
       </c>
-      <c r="H6" s="28">
+      <c r="I6" s="2">
         <f>raw_data!AB7</f>
         <v>275000</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="30">
+    <row r="7" spans="1:9">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="15">
         <f>raw_data!D8</f>
         <v>1</v>
       </c>
-      <c r="B7" s="28">
+      <c r="C7" s="2">
         <f>raw_data!V8</f>
         <v>2</v>
       </c>
-      <c r="C7" s="28">
+      <c r="D7" s="2">
         <f>raw_data!W8</f>
         <v>-0.16489999999999999</v>
       </c>
-      <c r="D7" s="31">
+      <c r="E7" s="14">
         <f>raw_data!X8</f>
         <v>1</v>
       </c>
-      <c r="E7" s="28">
+      <c r="F7" s="2">
         <f>raw_data!Y8</f>
         <v>620000</v>
       </c>
-      <c r="F7" s="28">
+      <c r="G7" s="2">
         <f>raw_data!Z8</f>
         <v>550000</v>
       </c>
-      <c r="G7" s="28">
+      <c r="H7" s="2">
         <f>raw_data!AA8</f>
         <v>480000</v>
       </c>
-      <c r="H7" s="28">
+      <c r="I7" s="2">
         <f>raw_data!AB8</f>
         <v>400000</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="30">
+    <row r="8" spans="1:9">
+      <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="15">
         <f>raw_data!D9</f>
         <v>1</v>
       </c>
-      <c r="B8" s="28">
+      <c r="C8" s="2">
         <f>raw_data!V9</f>
         <v>2.8250000000000002</v>
       </c>
-      <c r="C8" s="28">
+      <c r="D8" s="2">
         <f>raw_data!W9</f>
         <v>0.1414</v>
       </c>
-      <c r="D8" s="31">
+      <c r="E8" s="14">
         <f>raw_data!X9</f>
         <v>1</v>
       </c>
-      <c r="E8" s="28">
+      <c r="F8" s="2">
         <f>raw_data!Y9</f>
         <v>1250000</v>
       </c>
-      <c r="F8" s="28">
+      <c r="G8" s="2">
         <f>raw_data!Z9</f>
         <v>900000</v>
       </c>
-      <c r="G8" s="28">
+      <c r="H8" s="2">
         <f>raw_data!AA9</f>
         <v>670000</v>
       </c>
-      <c r="H8" s="28">
+      <c r="I8" s="2">
         <f>raw_data!AB9</f>
         <v>565000</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="30">
+    <row r="9" spans="1:9">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="15">
         <f>raw_data!D10</f>
         <v>1</v>
       </c>
-      <c r="B9" s="28">
+      <c r="C9" s="2">
         <f>raw_data!V10</f>
         <v>0.75</v>
       </c>
-      <c r="C9" s="28">
+      <c r="D9" s="2">
         <f>raw_data!W10</f>
         <v>12.538500000000001</v>
       </c>
-      <c r="D9" s="31">
+      <c r="E9" s="14">
         <f>raw_data!X10</f>
         <v>1</v>
       </c>
-      <c r="E9" s="28">
+      <c r="F9" s="2">
         <f>raw_data!Y10</f>
         <v>870610</v>
       </c>
-      <c r="F9" s="28">
+      <c r="G9" s="2">
         <f>raw_data!Z10</f>
         <v>400000</v>
       </c>
-      <c r="G9" s="28">
+      <c r="H9" s="2">
         <f>raw_data!AA10</f>
         <v>269000</v>
       </c>
-      <c r="H9" s="28">
+      <c r="I9" s="2">
         <f>raw_data!AB10</f>
         <v>150000</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="30">
+    <row r="10" spans="1:9">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="15">
         <f>raw_data!D11</f>
         <v>1</v>
       </c>
-      <c r="B10" s="28">
+      <c r="C10" s="2">
         <f>raw_data!V11</f>
         <v>0.61499999999999999</v>
       </c>
-      <c r="C10" s="28">
+      <c r="D10" s="2">
         <f>raw_data!W11</f>
         <v>-8.0999999999999996E-3</v>
       </c>
-      <c r="D10" s="31">
+      <c r="E10" s="14">
         <f>raw_data!X11</f>
         <v>1</v>
       </c>
-      <c r="E10" s="28">
+      <c r="F10" s="2">
         <f>raw_data!Y11</f>
         <v>795000</v>
       </c>
-      <c r="F10" s="28">
+      <c r="G10" s="2">
         <f>raw_data!Z11</f>
         <v>710000</v>
       </c>
-      <c r="G10" s="28">
+      <c r="H10" s="2">
         <f>raw_data!AA11</f>
         <v>655000</v>
       </c>
-      <c r="H10" s="28">
+      <c r="I10" s="2">
         <f>raw_data!AB11</f>
         <v>615000</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="30">
+    <row r="11" spans="1:9">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="15">
         <f>raw_data!D12</f>
         <v>1</v>
       </c>
-      <c r="B11" s="28">
+      <c r="C11" s="2">
         <f>raw_data!V12</f>
         <v>0.67800000000000005</v>
       </c>
-      <c r="C11" s="28">
+      <c r="D11" s="2">
         <f>raw_data!W12</f>
         <v>3.5099999999999999E-2</v>
       </c>
-      <c r="D11" s="31">
+      <c r="E11" s="14">
         <f>raw_data!X12</f>
         <v>1</v>
       </c>
-      <c r="E11" s="28">
+      <c r="F11" s="2">
         <f>raw_data!Y12</f>
         <v>829000</v>
       </c>
-      <c r="F11" s="28">
+      <c r="G11" s="2">
         <f>raw_data!Z12</f>
         <v>790000</v>
       </c>
-      <c r="G11" s="28">
+      <c r="H11" s="2">
         <f>raw_data!AA12</f>
         <v>725000</v>
       </c>
-      <c r="H11" s="28">
+      <c r="I11" s="2">
         <f>raw_data!AB12</f>
         <v>678000</v>
       </c>
@@ -3464,384 +3554,420 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D305217F-6C26-4A1F-AC1F-AEDFC3CA9CD4}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="C1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="E1" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="30">
+    <row r="2" spans="1:9">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="15">
         <f>raw_data!D3</f>
         <v>1</v>
       </c>
-      <c r="B2" s="28">
+      <c r="C2" s="2">
         <f>raw_data!AC3</f>
         <v>22</v>
       </c>
-      <c r="C2" s="28">
+      <c r="D2" s="2">
         <f>raw_data!AD3</f>
         <v>1</v>
       </c>
-      <c r="D2" s="31">
+      <c r="E2" s="14">
         <f>raw_data!AE3</f>
         <v>1</v>
       </c>
-      <c r="E2" s="28">
+      <c r="F2" s="2">
         <f>raw_data!AF3</f>
         <v>9800000</v>
       </c>
-      <c r="F2" s="28">
+      <c r="G2" s="2">
         <f>raw_data!AG3</f>
         <v>6000000</v>
       </c>
-      <c r="G2" s="28">
+      <c r="H2" s="2">
         <f>raw_data!AH3</f>
         <v>5000000</v>
       </c>
-      <c r="H2" s="28">
+      <c r="I2" s="2">
         <f>raw_data!AI3</f>
         <v>4400000</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="30">
+    <row r="3" spans="1:9">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="15">
         <f>raw_data!D4</f>
         <v>1</v>
       </c>
-      <c r="B3" s="28">
+      <c r="C3" s="2">
         <f>raw_data!AC4</f>
         <v>11.5</v>
       </c>
-      <c r="C3" s="28">
+      <c r="D3" s="2">
         <f>raw_data!AD4</f>
         <v>0.39389999999999997</v>
       </c>
-      <c r="D3" s="31">
+      <c r="E3" s="14">
         <f>raw_data!AE4</f>
         <v>1</v>
       </c>
-      <c r="E3" s="28">
+      <c r="F3" s="2">
         <f>raw_data!AF4</f>
         <v>4800000</v>
       </c>
-      <c r="F3" s="28">
+      <c r="G3" s="2">
         <f>raw_data!AG4</f>
         <v>3300000</v>
       </c>
-      <c r="G3" s="28">
+      <c r="H3" s="2">
         <f>raw_data!AH4</f>
         <v>2990000</v>
       </c>
-      <c r="H3" s="28">
+      <c r="I3" s="2">
         <f>raw_data!AI4</f>
         <v>2300000</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="30">
+    <row r="4" spans="1:9">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="15">
         <f>raw_data!D5</f>
         <v>1</v>
       </c>
-      <c r="B4" s="28">
+      <c r="C4" s="2">
         <f>raw_data!AC5</f>
         <v>10</v>
       </c>
-      <c r="C4" s="28">
+      <c r="D4" s="2">
         <f>raw_data!AD5</f>
         <v>6</v>
       </c>
-      <c r="D4" s="31">
+      <c r="E4" s="14">
         <f>raw_data!AE5</f>
         <v>1</v>
       </c>
-      <c r="E4" s="28">
+      <c r="F4" s="2">
         <f>raw_data!AF5</f>
         <v>5000000</v>
       </c>
-      <c r="F4" s="28">
+      <c r="G4" s="2">
         <f>raw_data!AG5</f>
         <v>4000000</v>
       </c>
-      <c r="G4" s="28">
+      <c r="H4" s="2">
         <f>raw_data!AH5</f>
         <v>3200000</v>
       </c>
-      <c r="H4" s="28">
+      <c r="I4" s="2">
         <f>raw_data!AI5</f>
         <v>2000000</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="30">
+    <row r="5" spans="1:9">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="15">
         <f>raw_data!D6</f>
         <v>1</v>
       </c>
-      <c r="B5" s="28">
+      <c r="C5" s="2">
         <f>raw_data!AC6</f>
         <v>20.5</v>
       </c>
-      <c r="C5" s="28">
+      <c r="D5" s="2">
         <f>raw_data!AD6</f>
         <v>1.1026</v>
       </c>
-      <c r="D5" s="31">
+      <c r="E5" s="14">
         <f>raw_data!AE6</f>
         <v>1</v>
       </c>
-      <c r="E5" s="28">
+      <c r="F5" s="2">
         <f>raw_data!AF6</f>
         <v>8800000</v>
       </c>
-      <c r="F5" s="28">
+      <c r="G5" s="2">
         <f>raw_data!AG6</f>
         <v>5100000</v>
       </c>
-      <c r="G5" s="28">
+      <c r="H5" s="2">
         <f>raw_data!AH6</f>
         <v>4700000</v>
       </c>
-      <c r="H5" s="28">
+      <c r="I5" s="2">
         <f>raw_data!AI6</f>
         <v>4100000</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="30">
+    <row r="6" spans="1:9">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="15">
         <f>raw_data!D7</f>
         <v>1</v>
       </c>
-      <c r="B6" s="28">
+      <c r="C6" s="2">
         <f>raw_data!AC7</f>
         <v>1.5</v>
       </c>
-      <c r="C6" s="28">
+      <c r="D6" s="2">
         <f>raw_data!AD7</f>
         <v>9.0899999999999995E-2</v>
       </c>
-      <c r="D6" s="31">
+      <c r="E6" s="14">
         <f>raw_data!AE7</f>
         <v>1</v>
       </c>
-      <c r="E6" s="28">
+      <c r="F6" s="2">
         <f>raw_data!AF7</f>
         <v>480000</v>
       </c>
-      <c r="F6" s="28">
+      <c r="G6" s="2">
         <f>raw_data!AG7</f>
         <v>400000</v>
       </c>
-      <c r="G6" s="28">
+      <c r="H6" s="2">
         <f>raw_data!AH7</f>
         <v>350000</v>
       </c>
-      <c r="H6" s="28">
+      <c r="I6" s="2">
         <f>raw_data!AI7</f>
         <v>300000</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="30">
+    <row r="7" spans="1:9">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="15">
         <f>raw_data!D8</f>
         <v>1</v>
       </c>
-      <c r="B7" s="28">
+      <c r="C7" s="2">
         <f>raw_data!AC8</f>
         <v>1.9750000000000001</v>
       </c>
-      <c r="C7" s="28">
+      <c r="D7" s="2">
         <f>raw_data!AD8</f>
         <v>-1.2500000000000001E-2</v>
       </c>
-      <c r="D7" s="31">
+      <c r="E7" s="14">
         <f>raw_data!AE8</f>
         <v>1</v>
       </c>
-      <c r="E7" s="28">
+      <c r="F7" s="2">
         <f>raw_data!AF8</f>
         <v>600000</v>
       </c>
-      <c r="F7" s="28">
+      <c r="G7" s="2">
         <f>raw_data!AG8</f>
         <v>510000</v>
       </c>
-      <c r="G7" s="28">
+      <c r="H7" s="2">
         <f>raw_data!AH8</f>
         <v>470000</v>
       </c>
-      <c r="H7" s="28">
+      <c r="I7" s="2">
         <f>raw_data!AI8</f>
         <v>395000</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="30">
+    <row r="8" spans="1:9">
+      <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="15">
         <f>raw_data!D9</f>
         <v>1</v>
       </c>
-      <c r="B8" s="28">
+      <c r="C8" s="2">
         <f>raw_data!AC9</f>
         <v>3.2149999999999999</v>
       </c>
-      <c r="C8" s="28">
+      <c r="D8" s="2">
         <f>raw_data!AD9</f>
         <v>0.1381</v>
       </c>
-      <c r="D8" s="31">
+      <c r="E8" s="14">
         <f>raw_data!AE9</f>
         <v>1</v>
       </c>
-      <c r="E8" s="28">
+      <c r="F8" s="2">
         <f>raw_data!AF9</f>
         <v>1400000</v>
       </c>
-      <c r="F8" s="28">
+      <c r="G8" s="2">
         <f>raw_data!AG9</f>
         <v>1050000</v>
       </c>
-      <c r="G8" s="28">
+      <c r="H8" s="2">
         <f>raw_data!AH9</f>
         <v>760000</v>
       </c>
-      <c r="H8" s="28">
+      <c r="I8" s="2">
         <f>raw_data!AI9</f>
         <v>643000</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="30">
+    <row r="9" spans="1:9">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="15">
         <f>raw_data!D10</f>
         <v>1</v>
       </c>
-      <c r="B9" s="28">
+      <c r="C9" s="2">
         <f>raw_data!AC10</f>
         <v>1.89</v>
       </c>
-      <c r="C9" s="28">
+      <c r="D9" s="2">
         <f>raw_data!AD10</f>
         <v>1.52</v>
       </c>
-      <c r="D9" s="31">
+      <c r="E9" s="14">
         <f>raw_data!AE10</f>
         <v>1</v>
       </c>
-      <c r="E9" s="28">
+      <c r="F9" s="2">
         <f>raw_data!AF10</f>
         <v>800000</v>
       </c>
-      <c r="F9" s="28">
+      <c r="G9" s="2">
         <f>raw_data!AG10</f>
         <v>610000</v>
       </c>
-      <c r="G9" s="28">
+      <c r="H9" s="2">
         <f>raw_data!AH10</f>
         <v>432000</v>
       </c>
-      <c r="H9" s="28">
+      <c r="I9" s="2">
         <f>raw_data!AI10</f>
         <v>378000</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="30">
+    <row r="10" spans="1:9">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="15">
         <f>raw_data!D11</f>
         <v>1</v>
       </c>
-      <c r="B10" s="28">
+      <c r="C10" s="2">
         <f>raw_data!AC11</f>
         <v>0.65</v>
       </c>
-      <c r="C10" s="28">
+      <c r="D10" s="2">
         <f>raw_data!AD11</f>
         <v>5.6899999999999999E-2</v>
       </c>
-      <c r="D10" s="31">
+      <c r="E10" s="14">
         <f>raw_data!AE11</f>
         <v>1</v>
       </c>
-      <c r="E10" s="28">
+      <c r="F10" s="2">
         <f>raw_data!AF11</f>
         <v>820000</v>
       </c>
-      <c r="F10" s="28">
+      <c r="G10" s="2">
         <f>raw_data!AG11</f>
         <v>780000</v>
       </c>
-      <c r="G10" s="28">
+      <c r="H10" s="2">
         <f>raw_data!AH11</f>
         <v>720000</v>
       </c>
-      <c r="H10" s="28">
+      <c r="I10" s="2">
         <f>raw_data!AI11</f>
         <v>650000</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="30">
+    <row r="11" spans="1:9">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="15">
         <f>raw_data!D12</f>
         <v>1</v>
       </c>
-      <c r="B11" s="28">
+      <c r="C11" s="2">
         <f>raw_data!AC12</f>
         <v>0.69</v>
       </c>
-      <c r="C11" s="28">
+      <c r="D11" s="2">
         <f>raw_data!AD12</f>
         <v>1.77E-2</v>
       </c>
-      <c r="D11" s="31">
+      <c r="E11" s="14">
         <f>raw_data!AE12</f>
         <v>1</v>
       </c>
-      <c r="E11" s="28">
+      <c r="F11" s="2">
         <f>raw_data!AF12</f>
         <v>831000</v>
       </c>
-      <c r="F11" s="28">
+      <c r="G11" s="2">
         <f>raw_data!AG12</f>
         <v>800000</v>
       </c>
-      <c r="G11" s="28">
+      <c r="H11" s="2">
         <f>raw_data!AH12</f>
         <v>750000</v>
       </c>
-      <c r="H11" s="28">
+      <c r="I11" s="2">
         <f>raw_data!AI12</f>
         <v>690000</v>
       </c>

</xml_diff>

<commit_message>
Minor changes on stock_data.xlsx.
</commit_message>
<xml_diff>
--- a/Data/stock_data.xlsx
+++ b/Data/stock_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\NTUT\Other\113IFM_camp\IFM_camp_bot\Bot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D15805C-FDCD-46C1-8699-973CC6907711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F8F17F-40D0-45CD-B174-7E07ED946401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F8FD49BE-BC86-4C92-8F4D-99B84D176403}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F8FD49BE-BC86-4C92-8F4D-99B84D176403}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_data" sheetId="2" r:id="rId1"/>
@@ -55,10 +55,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>industry</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>奕為創</t>
   </si>
   <si>
@@ -189,6 +185,10 @@
   </si>
   <si>
     <t>adjust_ratio</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sector</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -717,9 +717,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A5B1930-18B5-46DE-91AC-AB66E4E6FDB4}">
   <dimension ref="A1:AI12"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G21" sqref="G21"/>
+      <selection pane="topRight" activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -770,22 +770,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G1" s="22" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I1" s="20"/>
       <c r="J1" s="20"/>
@@ -794,7 +794,7 @@
       <c r="M1" s="20"/>
       <c r="N1" s="21"/>
       <c r="O1" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P1" s="20"/>
       <c r="Q1" s="20"/>
@@ -803,7 +803,7 @@
       <c r="T1" s="20"/>
       <c r="U1" s="21"/>
       <c r="V1" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="W1" s="20"/>
       <c r="X1" s="20"/>
@@ -812,7 +812,7 @@
       <c r="AA1" s="20"/>
       <c r="AB1" s="21"/>
       <c r="AC1" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AD1" s="20"/>
       <c r="AE1" s="20"/>
@@ -830,99 +830,99 @@
       <c r="F2" s="24"/>
       <c r="G2" s="22"/>
       <c r="H2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="O2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="R2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="P2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="T2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="U2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="U2" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="V2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="W2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="X2" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Z2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="AA2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AB2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AB2" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="AC2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AD2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE2" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AG2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AH2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AH2" s="4" t="s">
+      <c r="AI2" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="AI2" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:35" ht="15.75">
       <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="C3" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="15">
         <v>1</v>
@@ -1031,13 +1031,13 @@
     </row>
     <row r="4" spans="1:35" ht="15.75">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="15">
         <v>1</v>
@@ -1146,13 +1146,13 @@
     </row>
     <row r="5" spans="1:35" ht="15.75">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" s="15">
         <v>1</v>
@@ -1261,13 +1261,13 @@
     </row>
     <row r="6" spans="1:35" ht="15.75">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="15">
         <v>1</v>
@@ -1376,13 +1376,13 @@
     </row>
     <row r="7" spans="1:35" ht="15.75">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="15">
         <v>1</v>
@@ -1491,13 +1491,13 @@
     </row>
     <row r="8" spans="1:35" ht="15.75">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="15">
         <v>1</v>
@@ -1606,13 +1606,13 @@
     </row>
     <row r="9" spans="1:35" ht="15.75">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" s="15">
         <v>1</v>
@@ -1721,13 +1721,13 @@
     </row>
     <row r="10" spans="1:35" ht="15.75">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="15">
         <v>1</v>
@@ -1836,13 +1836,13 @@
     </row>
     <row r="11" spans="1:35" ht="15.75">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="15">
         <v>1</v>
@@ -1951,13 +1951,13 @@
     </row>
     <row r="12" spans="1:35" ht="15.75">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="15">
         <v>1</v>
@@ -2087,8 +2087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E8A576-3FE2-48FD-990C-850FE256943E}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2107,21 +2107,21 @@
         <v>2</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="C2" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2">
         <f>raw_data!E3</f>
@@ -2130,13 +2130,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="2">
         <f>raw_data!E4</f>
@@ -2145,13 +2145,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="2">
         <f>raw_data!E5</f>
@@ -2160,13 +2160,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" s="2">
         <f>raw_data!E6</f>
@@ -2175,13 +2175,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="2">
         <f>raw_data!E7</f>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="2">
         <f>raw_data!E8</f>
@@ -2205,13 +2205,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="2">
         <f>raw_data!E9</f>
@@ -2220,13 +2220,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" s="2">
         <f>raw_data!E10</f>
@@ -2235,13 +2235,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="2">
         <f>raw_data!E11</f>
@@ -2250,13 +2250,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="2">
         <f>raw_data!E12</f>
@@ -2291,28 +2291,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2686,28 +2686,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -3078,28 +3078,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -3470,28 +3470,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:8">

</xml_diff>